<commit_message>
Änderung für Parallelisierung der Feldprüfung
</commit_message>
<xml_diff>
--- a/src/main/resources/base/owfw7/TestCustomerPartNumber.xlsx
+++ b/src/main/resources/base/owfw7/TestCustomerPartNumber.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkellermann\Documents\git\importitnew\src\main\resources\base\owfw7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\abas\git\importitnew\src\main\resources\base\owfw7\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB94B0A3-F3AB-4B41-988A-A97EC91975D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="-465" windowWidth="0" windowHeight="17685"/>
+    <workbookView xWindow="2745" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>BARVERKAUF</t>
   </si>
@@ -40,11 +41,17 @@
   <si>
     <t>test</t>
   </si>
+  <si>
+    <t>BARVERKAUF 1</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -432,11 +439,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -489,6 +496,182 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10027</v>
+      </c>
+      <c r="B5">
+        <v>50000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10027</v>
+      </c>
+      <c r="B6">
+        <v>70003</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10026</v>
+      </c>
+      <c r="B7">
+        <v>50000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10026</v>
+      </c>
+      <c r="B8">
+        <v>70003</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>10028</v>
+      </c>
+      <c r="B9">
+        <v>50000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10028</v>
+      </c>
+      <c r="B10">
+        <v>70003</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10027</v>
+      </c>
+      <c r="B11">
+        <v>50000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10027</v>
+      </c>
+      <c r="B12">
+        <v>70003</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10026</v>
+      </c>
+      <c r="B13">
+        <v>50000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10026</v>
+      </c>
+      <c r="B14">
+        <v>70003</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>10028</v>
+      </c>
+      <c r="B15">
+        <v>50000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>10028</v>
+      </c>
+      <c r="B16">
+        <v>70003</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>10027</v>
+      </c>
+      <c r="B17">
+        <v>50000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>10027</v>
+      </c>
+      <c r="B18">
+        <v>70003</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10026</v>
+      </c>
+      <c r="B19">
+        <v>50000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>10026</v>
+      </c>
+      <c r="B20">
+        <v>70003</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -498,7 +681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -512,7 +695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>